<commit_message>
add RMSE percentage for Morocco soil and try EFAST
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/sensitivity_RMSE_Morocco_soil.xlsx
+++ b/heliostrome/jip_project/results/sensitivity_RMSE_Morocco_soil.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>RMSE</t>
+          <t>Yield RMSE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Yield RMSE Percentage</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Water Used RMSE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Water Used RMSE Percentage</t>
         </is>
       </c>
     </row>
@@ -454,6 +469,15 @@
       <c r="B2" t="n">
         <v>1.083337404366888</v>
       </c>
+      <c r="C2" t="n">
+        <v>50.66685706577445</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -464,6 +488,15 @@
       <c r="B3" t="n">
         <v>1.469644101978667</v>
       </c>
+      <c r="C3" t="n">
+        <v>68.73412415407923</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -474,6 +507,15 @@
       <c r="B4" t="n">
         <v>1.472856312244285</v>
       </c>
+      <c r="C4" t="n">
+        <v>68.88435675727116</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -484,6 +526,15 @@
       <c r="B5" t="n">
         <v>1.467127531340894</v>
       </c>
+      <c r="C5" t="n">
+        <v>68.61642608117414</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -492,7 +543,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.536866645809523</v>
+        <v>1.536866645809522</v>
+      </c>
+      <c r="C6" t="n">
+        <v>71.87807081939918</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -504,6 +564,15 @@
       <c r="B7" t="n">
         <v>1.351816408424473</v>
       </c>
+      <c r="C7" t="n">
+        <v>63.22341356323691</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -514,6 +583,15 @@
       <c r="B8" t="n">
         <v>1.372321928882388</v>
       </c>
+      <c r="C8" t="n">
+        <v>64.18244098157632</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -522,7 +600,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.261615158411221</v>
+        <v>1.261615158411222</v>
+      </c>
+      <c r="C9" t="n">
+        <v>59.00477048569406</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -534,6 +621,15 @@
       <c r="B10" t="n">
         <v>2.202618881439304</v>
       </c>
+      <c r="C10" t="n">
+        <v>103.0147907626998</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -544,6 +640,15 @@
       <c r="B11" t="n">
         <v>1.647594920961394</v>
       </c>
+      <c r="C11" t="n">
+        <v>77.05674707265599</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -552,7 +657,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.775887473276424</v>
+        <v>1.775887473276425</v>
+      </c>
+      <c r="C12" t="n">
+        <v>83.05689105785127</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -564,6 +678,15 @@
       <c r="B13" t="n">
         <v>1.564843846393799</v>
       </c>
+      <c r="C13" t="n">
+        <v>73.1865429698023</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -574,6 +697,15 @@
       <c r="B14" t="n">
         <v>1.896310546809407</v>
       </c>
+      <c r="C14" t="n">
+        <v>88.68898557385536</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -583,6 +715,15 @@
       </c>
       <c r="B15" t="n">
         <v>1.868033900175231</v>
+      </c>
+      <c r="C15" t="n">
+        <v>87.36650856204157</v>
+      </c>
+      <c r="D15" t="n">
+        <v>10.88214375165017</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6.691285801985544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>